<commit_message>
Improved version of sprint back log
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A613AFDB-AC65-4A60-B71C-A2B155251F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAD35FF-6B27-4CA7-B5AF-2FAF95BA3F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B5F37A8-96CD-4EC4-AE7C-68DE6E3FF2F8}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
-  <si>
-    <t>ToDo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>In Progress</t>
   </si>
@@ -56,49 +53,70 @@
     <t>Martim Costa</t>
   </si>
   <si>
-    <t xml:space="preserve"> Martim Costa</t>
-  </si>
-  <si>
     <t>Pedro Arruda</t>
   </si>
   <si>
     <t>Bernardo Carvalho</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bernardo Carvalho</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pedro Arruda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ana Gadelha</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rodrigo Mesquita</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review each others design patterns </t>
-  </si>
-  <si>
     <t>Identify 3 code smells</t>
   </si>
   <si>
     <t>Identify 3 design paterns</t>
   </si>
   <si>
-    <t xml:space="preserve">Identify 3 design paterns </t>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Done By</t>
+  </si>
+  <si>
+    <t>Ana Gadelha</t>
+  </si>
+  <si>
+    <t>Rodrigo Mesquita</t>
+  </si>
+  <si>
+    <t>Bernardo carvalho</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Review each others design patterns</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,13 +176,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14574383-ECA1-4DA8-ADE6-D7F9BAD5BBB9}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,157 +516,200 @@
     <col min="2" max="2" width="34.44140625" customWidth="1"/>
     <col min="3" max="3" width="30.88671875" customWidth="1"/>
     <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scrum board and work breakdown done. Sprint back log updated
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAD35FF-6B27-4CA7-B5AF-2FAF95BA3F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0A5946-E47E-4740-AE76-CD21853EE184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B5F37A8-96CD-4EC4-AE7C-68DE6E3FF2F8}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>